<commit_message>
Updte GetVoteSummaries and SaveQSet (QSet table add column)
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="164">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -487,6 +487,27 @@
   </si>
   <si>
     <t>The BranchId not found.</t>
+  </si>
+  <si>
+    <t>SaveQSet</t>
+  </si>
+  <si>
+    <t>QSet Id is not found.</t>
+  </si>
+  <si>
+    <t>QSet is already used in vote table.</t>
+  </si>
+  <si>
+    <t>Begin Date and/or End Date should not be null.</t>
+  </si>
+  <si>
+    <t>Display Mode is null or value is not in 0 to 1.</t>
+  </si>
+  <si>
+    <t>Begin Date should less than End Date.</t>
+  </si>
+  <si>
+    <t>Begin Date or End Date is overlap with another Question Set.</t>
   </si>
 </sst>
 </file>
@@ -830,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2306,153 +2327,175 @@
       <c r="A143">
         <v>1401</v>
       </c>
+      <c r="B143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C143" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
         <v>1402</v>
       </c>
+      <c r="B144" t="s">
+        <v>97</v>
+      </c>
+      <c r="C144" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145">
         <v>1403</v>
       </c>
+      <c r="B145" t="s">
+        <v>158</v>
+      </c>
+      <c r="C145" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146">
         <v>1404</v>
       </c>
+      <c r="B146" t="s">
+        <v>159</v>
+      </c>
+      <c r="C146" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147">
         <v>1405</v>
       </c>
+      <c r="B147" t="s">
+        <v>160</v>
+      </c>
+      <c r="C147" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148">
         <v>1406</v>
       </c>
+      <c r="B148" t="s">
+        <v>161</v>
+      </c>
+      <c r="C148" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149">
+        <v>1407</v>
+      </c>
+      <c r="B149" t="s">
+        <v>162</v>
+      </c>
+      <c r="C149" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="A150">
+        <v>1408</v>
+      </c>
+      <c r="B150" t="s">
+        <v>163</v>
+      </c>
+      <c r="C150" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153">
-        <v>1503</v>
+        <v>1409</v>
+      </c>
+      <c r="C151" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154">
-        <v>1504</v>
-      </c>
+      <c r="A154" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
     </row>
     <row r="155" spans="1:3">
       <c r="A155">
-        <v>1505</v>
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156">
+        <v>1502</v>
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
+      <c r="A157">
+        <v>1503</v>
+      </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158">
-        <v>1601</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160">
-        <v>1603</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161">
-        <v>1604</v>
-      </c>
+      <c r="A161" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
     </row>
     <row r="162" spans="1:3">
       <c r="A162">
-        <v>1605</v>
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>1602</v>
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+      <c r="A164">
+        <v>1603</v>
+      </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>1701</v>
-      </c>
-      <c r="B165" t="s">
-        <v>90</v>
-      </c>
-      <c r="C165" t="s">
-        <v>141</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>1702</v>
-      </c>
-      <c r="B166" t="s">
-        <v>108</v>
-      </c>
-      <c r="C166" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167">
-        <v>1703</v>
-      </c>
-      <c r="B167" t="s">
-        <v>104</v>
-      </c>
-      <c r="C167" t="s">
-        <v>141</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168">
-        <v>1704</v>
-      </c>
-      <c r="B168" t="s">
-        <v>126</v>
-      </c>
-      <c r="C168" t="s">
-        <v>141</v>
-      </c>
+      <c r="A168" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>1705</v>
+        <v>1701</v>
       </c>
       <c r="B169" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="C169" t="s">
         <v>141</v>
@@ -2460,10 +2503,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>1706</v>
+        <v>1702</v>
       </c>
       <c r="B170" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="C170" t="s">
         <v>141</v>
@@ -2471,10 +2514,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>1707</v>
+        <v>1703</v>
       </c>
       <c r="B171" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C171" t="s">
         <v>141</v>
@@ -2482,146 +2525,190 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="B172" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C172" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="173" spans="1:3">
+      <c r="A173">
+        <v>1705</v>
+      </c>
+      <c r="B173" t="s">
+        <v>132</v>
+      </c>
+      <c r="C173" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
+      <c r="A174">
+        <v>1706</v>
+      </c>
+      <c r="B174" t="s">
+        <v>140</v>
+      </c>
+      <c r="C174" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175">
-        <v>1801</v>
+        <v>1707</v>
       </c>
       <c r="B175" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C175" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176">
-        <v>1802</v>
+        <v>1708</v>
       </c>
       <c r="B176" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C176" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>1901</v>
+        <v>1801</v>
       </c>
       <c r="B179" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C179" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180">
+        <v>1802</v>
+      </c>
+      <c r="B180" t="s">
+        <v>148</v>
+      </c>
+      <c r="C180" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182">
-        <v>2001</v>
-      </c>
-      <c r="B182" t="s">
-        <v>152</v>
-      </c>
-      <c r="C182" t="s">
-        <v>151</v>
-      </c>
+      <c r="A182" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
     </row>
     <row r="183" spans="1:3">
       <c r="A183">
-        <v>2002</v>
+        <v>1901</v>
       </c>
       <c r="B183" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C183" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184">
-        <v>2003</v>
-      </c>
-      <c r="B184" t="s">
-        <v>154</v>
-      </c>
-      <c r="C184" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185">
-        <v>2004</v>
-      </c>
-      <c r="B185" t="s">
-        <v>155</v>
-      </c>
-      <c r="C185" t="s">
-        <v>151</v>
-      </c>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="B186" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C186" t="s">
         <v>151</v>
       </c>
     </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>2002</v>
+      </c>
+      <c r="B187" t="s">
+        <v>153</v>
+      </c>
+      <c r="C187" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>2003</v>
+      </c>
+      <c r="B188" t="s">
+        <v>154</v>
+      </c>
+      <c r="C188" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>2004</v>
+      </c>
+      <c r="B189" t="s">
+        <v>155</v>
+      </c>
+      <c r="C189" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>2005</v>
+      </c>
+      <c r="B190" t="s">
+        <v>156</v>
+      </c>
+      <c r="C190" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A174:C174"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A181:C181"/>
-    <mergeCell ref="A157:C157"/>
-    <mergeCell ref="A164:C164"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A150:C150"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A154:C154"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="A185:C185"/>
+    <mergeCell ref="A161:C161"/>
+    <mergeCell ref="A168:C168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Add db Script GetRawVotes and Error Message
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="168">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -508,6 +508,18 @@
   </si>
   <si>
     <t>Begin Date or End Date is overlap with another Question Set.</t>
+  </si>
+  <si>
+    <t>GetRawVotes</t>
+  </si>
+  <si>
+    <t>QSeq cannot be null or less than 1.</t>
+  </si>
+  <si>
+    <t>LangId Is Null Or Empty String.</t>
+  </si>
+  <si>
+    <t>Begin Date and End Date cannot be null.</t>
   </si>
 </sst>
 </file>
@@ -851,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2687,28 +2699,91 @@
         <v>151</v>
       </c>
     </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>2101</v>
+      </c>
+      <c r="B193" t="s">
+        <v>152</v>
+      </c>
+      <c r="C193" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194">
+        <v>2102</v>
+      </c>
+      <c r="B194" t="s">
+        <v>153</v>
+      </c>
+      <c r="C194" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195">
+        <v>2103</v>
+      </c>
+      <c r="B195" t="s">
+        <v>165</v>
+      </c>
+      <c r="C195" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196">
+        <v>2104</v>
+      </c>
+      <c r="B196" t="s">
+        <v>167</v>
+      </c>
+      <c r="C196" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197">
+        <v>2105</v>
+      </c>
+      <c r="B197" t="s">
+        <v>166</v>
+      </c>
+      <c r="C197" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="A192:C192"/>
+    <mergeCell ref="A178:C178"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="A185:C185"/>
+    <mergeCell ref="A161:C161"/>
+    <mergeCell ref="A168:C168"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A154:C154"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A88:C88"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A154:C154"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A182:C182"/>
-    <mergeCell ref="A185:C185"/>
-    <mergeCell ref="A161:C161"/>
-    <mergeCell ref="A168:C168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update SaveQSet, Add SaveQSetML script.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="176">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -520,6 +520,30 @@
   </si>
   <si>
     <t>Begin Date and End Date cannot be null.</t>
+  </si>
+  <si>
+    <t>SaveQSetML</t>
+  </si>
+  <si>
+    <t>No QSet match QSetId in specificed Customer Id.</t>
+  </si>
+  <si>
+    <t>Description(ML) already exists.</t>
+  </si>
+  <si>
+    <t>Description (default) already exists.</t>
+  </si>
+  <si>
+    <t>SaveQSlide</t>
+  </si>
+  <si>
+    <t>Question Set Id cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Question Text cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>QSetId is not found.</t>
   </si>
 </sst>
 </file>
@@ -863,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2427,363 +2451,518 @@
       <c r="A151">
         <v>1409</v>
       </c>
+      <c r="B151" t="s">
+        <v>86</v>
+      </c>
       <c r="C151" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>1410</v>
+      </c>
+      <c r="B152" t="s">
+        <v>89</v>
+      </c>
+      <c r="C152" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>1411</v>
+      </c>
+      <c r="B153" t="s">
+        <v>90</v>
+      </c>
+      <c r="C153" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
+      <c r="A154">
+        <v>1412</v>
+      </c>
+      <c r="B154" t="s">
+        <v>108</v>
+      </c>
+      <c r="C154" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155">
-        <v>1501</v>
+        <v>1413</v>
+      </c>
+      <c r="B155" t="s">
+        <v>153</v>
+      </c>
+      <c r="C155" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156">
-        <v>1502</v>
+        <v>1414</v>
+      </c>
+      <c r="B156" t="s">
+        <v>169</v>
+      </c>
+      <c r="C156" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157">
-        <v>1503</v>
+        <v>1415</v>
+      </c>
+      <c r="B157" t="s">
+        <v>170</v>
+      </c>
+      <c r="C157" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158">
-        <v>1504</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159">
-        <v>1505</v>
-      </c>
+        <v>1416</v>
+      </c>
+      <c r="B158" t="s">
+        <v>171</v>
+      </c>
+      <c r="C158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
+      <c r="A161">
+        <v>1501</v>
+      </c>
+      <c r="B161" t="s">
+        <v>90</v>
+      </c>
+      <c r="C161" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162">
-        <v>1601</v>
+        <v>1502</v>
+      </c>
+      <c r="B162" t="s">
+        <v>173</v>
+      </c>
+      <c r="C162" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>1602</v>
+        <v>1503</v>
+      </c>
+      <c r="B163" t="s">
+        <v>174</v>
+      </c>
+      <c r="C163" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>1603</v>
+        <v>1504</v>
+      </c>
+      <c r="B164" t="s">
+        <v>97</v>
+      </c>
+      <c r="C164" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>1604</v>
+        <v>1505</v>
+      </c>
+      <c r="B165" t="s">
+        <v>175</v>
+      </c>
+      <c r="C165" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>1605</v>
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167">
+        <v>1507</v>
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
+      <c r="A168">
+        <v>1508</v>
+      </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>1701</v>
-      </c>
-      <c r="B169" t="s">
-        <v>90</v>
-      </c>
-      <c r="C169" t="s">
-        <v>141</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>1702</v>
-      </c>
-      <c r="B170" t="s">
-        <v>108</v>
-      </c>
-      <c r="C170" t="s">
-        <v>141</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>1703</v>
-      </c>
-      <c r="B171" t="s">
-        <v>104</v>
-      </c>
-      <c r="C171" t="s">
-        <v>141</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>1704</v>
-      </c>
-      <c r="B172" t="s">
-        <v>126</v>
-      </c>
-      <c r="C172" t="s">
-        <v>141</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173">
-        <v>1705</v>
-      </c>
-      <c r="B173" t="s">
-        <v>132</v>
-      </c>
-      <c r="C173" t="s">
-        <v>141</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
-        <v>1706</v>
-      </c>
-      <c r="B174" t="s">
-        <v>140</v>
-      </c>
-      <c r="C174" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175">
-        <v>1707</v>
-      </c>
-      <c r="B175" t="s">
-        <v>142</v>
-      </c>
-      <c r="C175" t="s">
-        <v>141</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176">
-        <v>1708</v>
-      </c>
-      <c r="B176" t="s">
-        <v>143</v>
-      </c>
-      <c r="C176" t="s">
-        <v>141</v>
+      <c r="A176" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177">
+        <v>1601</v>
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+      <c r="A178">
+        <v>1602</v>
+      </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>1801</v>
-      </c>
-      <c r="B179" t="s">
-        <v>147</v>
-      </c>
-      <c r="C179" t="s">
-        <v>146</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180">
-        <v>1802</v>
-      </c>
-      <c r="B180" t="s">
-        <v>148</v>
-      </c>
-      <c r="C180" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181">
+        <v>1605</v>
+      </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183">
-        <v>1901</v>
-      </c>
-      <c r="B183" t="s">
-        <v>150</v>
-      </c>
-      <c r="C183" t="s">
-        <v>149</v>
+      <c r="A183" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B183" s="2"/>
+      <c r="C183" s="2"/>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>1701</v>
+      </c>
+      <c r="B184" t="s">
+        <v>90</v>
+      </c>
+      <c r="C184" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
+      <c r="A185">
+        <v>1702</v>
+      </c>
+      <c r="B185" t="s">
+        <v>108</v>
+      </c>
+      <c r="C185" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>2001</v>
+        <v>1703</v>
       </c>
       <c r="B186" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="C186" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>2002</v>
+        <v>1704</v>
       </c>
       <c r="B187" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="C187" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>2003</v>
+        <v>1705</v>
       </c>
       <c r="B188" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="C188" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>2004</v>
+        <v>1706</v>
       </c>
       <c r="B189" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C189" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>2005</v>
+        <v>1707</v>
       </c>
       <c r="B190" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C190" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>1708</v>
+      </c>
+      <c r="B191" t="s">
+        <v>143</v>
+      </c>
+      <c r="C191" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193">
-        <v>2101</v>
-      </c>
-      <c r="B193" t="s">
-        <v>152</v>
-      </c>
-      <c r="C193" t="s">
-        <v>164</v>
-      </c>
+      <c r="A193" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
     </row>
     <row r="194" spans="1:3">
       <c r="A194">
-        <v>2102</v>
+        <v>1801</v>
       </c>
       <c r="B194" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C194" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195">
+        <v>1802</v>
+      </c>
+      <c r="B195" t="s">
+        <v>148</v>
+      </c>
+      <c r="C195" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198">
+        <v>1901</v>
+      </c>
+      <c r="B198" t="s">
+        <v>150</v>
+      </c>
+      <c r="C198" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B200" s="2"/>
+      <c r="C200" s="2"/>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201">
+        <v>2001</v>
+      </c>
+      <c r="B201" t="s">
+        <v>152</v>
+      </c>
+      <c r="C201" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202">
+        <v>2002</v>
+      </c>
+      <c r="B202" t="s">
+        <v>153</v>
+      </c>
+      <c r="C202" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203">
+        <v>2003</v>
+      </c>
+      <c r="B203" t="s">
+        <v>154</v>
+      </c>
+      <c r="C203" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204">
+        <v>2004</v>
+      </c>
+      <c r="B204" t="s">
+        <v>155</v>
+      </c>
+      <c r="C204" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205">
+        <v>2005</v>
+      </c>
+      <c r="B205" t="s">
+        <v>156</v>
+      </c>
+      <c r="C205" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208">
+        <v>2101</v>
+      </c>
+      <c r="B208" t="s">
+        <v>152</v>
+      </c>
+      <c r="C208" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209">
+        <v>2102</v>
+      </c>
+      <c r="B209" t="s">
+        <v>153</v>
+      </c>
+      <c r="C209" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210">
         <v>2103</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B210" t="s">
         <v>165</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C210" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
-      <c r="A196">
+    <row r="211" spans="1:3">
+      <c r="A211">
         <v>2104</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B211" t="s">
         <v>167</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C211" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
-      <c r="A197">
+    <row r="212" spans="1:3">
+      <c r="A212">
         <v>2105</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B212" t="s">
         <v>166</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C212" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A192:C192"/>
-    <mergeCell ref="A178:C178"/>
-    <mergeCell ref="A182:C182"/>
-    <mergeCell ref="A185:C185"/>
-    <mergeCell ref="A161:C161"/>
-    <mergeCell ref="A168:C168"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A154:C154"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="A207:C207"/>
+    <mergeCell ref="A193:C193"/>
+    <mergeCell ref="A197:C197"/>
+    <mergeCell ref="A200:C200"/>
+    <mergeCell ref="A176:C176"/>
+    <mergeCell ref="A183:C183"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Error Message Excel File.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="183">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -429,9 +429,6 @@
     <t>Qslides</t>
   </si>
   <si>
-    <t>QslideItems</t>
-  </si>
-  <si>
     <t>Votes</t>
   </si>
   <si>
@@ -547,6 +544,27 @@
   </si>
   <si>
     <t>QSeq is not found.</t>
+  </si>
+  <si>
+    <t>SaveQSlideML</t>
+  </si>
+  <si>
+    <t>QSeq is null or less than zero.</t>
+  </si>
+  <si>
+    <t>No QSlide match QSetId and QSeq.</t>
+  </si>
+  <si>
+    <t>Question Text (ML) cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Question Text (ML) already exists.</t>
+  </si>
+  <si>
+    <t>QSlideItems</t>
+  </si>
+  <si>
+    <t>SaveQSlideItem</t>
   </si>
 </sst>
 </file>
@@ -890,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -940,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2320,7 +2338,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -2370,7 +2388,7 @@
         <v>90</v>
       </c>
       <c r="C143" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2381,7 +2399,7 @@
         <v>97</v>
       </c>
       <c r="C144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2389,10 +2407,10 @@
         <v>1403</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2400,10 +2418,10 @@
         <v>1404</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2411,10 +2429,10 @@
         <v>1405</v>
       </c>
       <c r="B147" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2422,10 +2440,10 @@
         <v>1406</v>
       </c>
       <c r="B148" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C148" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2433,10 +2451,10 @@
         <v>1407</v>
       </c>
       <c r="B149" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C149" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2444,10 +2462,10 @@
         <v>1408</v>
       </c>
       <c r="B150" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C150" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2458,7 +2476,7 @@
         <v>86</v>
       </c>
       <c r="C151" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2469,7 +2487,7 @@
         <v>89</v>
       </c>
       <c r="C152" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2480,7 +2498,7 @@
         <v>90</v>
       </c>
       <c r="C153" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2491,7 +2509,7 @@
         <v>108</v>
       </c>
       <c r="C154" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2499,10 +2517,10 @@
         <v>1413</v>
       </c>
       <c r="B155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C155" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2510,10 +2528,10 @@
         <v>1414</v>
       </c>
       <c r="B156" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C156" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2521,10 +2539,10 @@
         <v>1415</v>
       </c>
       <c r="B157" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C157" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2532,446 +2550,598 @@
         <v>1416</v>
       </c>
       <c r="B158" t="s">
-        <v>171</v>
+        <v>24</v>
       </c>
       <c r="C158" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>1417</v>
+      </c>
+      <c r="B159" t="s">
+        <v>170</v>
+      </c>
+      <c r="C159" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="2" t="s">
+      <c r="A160">
+        <v>1418</v>
+      </c>
+      <c r="B160" t="s">
+        <v>28</v>
+      </c>
+      <c r="C160" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161">
-        <v>1501</v>
-      </c>
-      <c r="B161" t="s">
-        <v>90</v>
-      </c>
-      <c r="C161" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162">
-        <v>1502</v>
-      </c>
-      <c r="B162" t="s">
-        <v>173</v>
-      </c>
-      <c r="C162" t="s">
-        <v>172</v>
-      </c>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="B163" t="s">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="C163" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B164" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="C164" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="B165" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C165" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="B166" t="s">
-        <v>176</v>
+        <v>97</v>
       </c>
       <c r="C166" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167">
-        <v>1507</v>
+        <v>1505</v>
+      </c>
+      <c r="B167" t="s">
+        <v>174</v>
+      </c>
+      <c r="C167" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168">
-        <v>1508</v>
+        <v>1506</v>
+      </c>
+      <c r="B168" t="s">
+        <v>175</v>
+      </c>
+      <c r="C168" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>1509</v>
+        <v>1507</v>
+      </c>
+      <c r="B169" t="s">
+        <v>86</v>
+      </c>
+      <c r="C169" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>1510</v>
+        <v>1508</v>
+      </c>
+      <c r="B170" t="s">
+        <v>89</v>
+      </c>
+      <c r="C170" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>1511</v>
+        <v>1509</v>
+      </c>
+      <c r="B171" t="s">
+        <v>90</v>
+      </c>
+      <c r="C171" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>1512</v>
+        <v>1510</v>
+      </c>
+      <c r="B172" t="s">
+        <v>108</v>
+      </c>
+      <c r="C172" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173">
-        <v>1513</v>
+        <v>1511</v>
+      </c>
+      <c r="B173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C173" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
+        <v>1512</v>
+      </c>
+      <c r="B174" t="s">
+        <v>168</v>
+      </c>
+      <c r="C174" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175">
+        <v>1513</v>
+      </c>
+      <c r="B175" t="s">
+        <v>177</v>
+      </c>
+      <c r="C175" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176">
         <v>1514</v>
       </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
+      <c r="B176" t="s">
+        <v>178</v>
+      </c>
+      <c r="C176" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>1601</v>
+        <v>1515</v>
+      </c>
+      <c r="B177" t="s">
+        <v>179</v>
+      </c>
+      <c r="C177" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179">
-        <v>1603</v>
+        <v>1516</v>
+      </c>
+      <c r="B178" t="s">
+        <v>180</v>
+      </c>
+      <c r="C178" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180">
-        <v>1604</v>
-      </c>
+      <c r="A180" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>1605</v>
+        <v>1601</v>
+      </c>
+      <c r="C181" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>1602</v>
+      </c>
+      <c r="C182" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
+      <c r="A183">
+        <v>1603</v>
+      </c>
+      <c r="C183" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>1701</v>
-      </c>
-      <c r="B184" t="s">
-        <v>90</v>
+        <v>1604</v>
       </c>
       <c r="C184" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185">
-        <v>1702</v>
-      </c>
-      <c r="B185" t="s">
-        <v>108</v>
+        <v>1605</v>
       </c>
       <c r="C185" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>1703</v>
-      </c>
-      <c r="B186" t="s">
-        <v>104</v>
-      </c>
-      <c r="C186" t="s">
-        <v>141</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>1704</v>
-      </c>
-      <c r="B187" t="s">
-        <v>126</v>
-      </c>
-      <c r="C187" t="s">
-        <v>141</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>1705</v>
-      </c>
-      <c r="B188" t="s">
-        <v>132</v>
-      </c>
-      <c r="C188" t="s">
-        <v>141</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>1706</v>
-      </c>
-      <c r="B189" t="s">
-        <v>140</v>
-      </c>
-      <c r="C189" t="s">
-        <v>141</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>1707</v>
-      </c>
-      <c r="B190" t="s">
-        <v>142</v>
-      </c>
-      <c r="C190" t="s">
-        <v>141</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191">
-        <v>1708</v>
-      </c>
-      <c r="B191" t="s">
-        <v>143</v>
-      </c>
-      <c r="C191" t="s">
-        <v>141</v>
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>1612</v>
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="A193">
+        <v>1613</v>
+      </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194">
-        <v>1801</v>
-      </c>
-      <c r="B194" t="s">
-        <v>147</v>
-      </c>
-      <c r="C194" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195">
-        <v>1802</v>
-      </c>
-      <c r="B195" t="s">
-        <v>148</v>
-      </c>
-      <c r="C195" t="s">
-        <v>146</v>
-      </c>
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
+      <c r="A197">
+        <v>1701</v>
+      </c>
+      <c r="B197" t="s">
+        <v>90</v>
+      </c>
+      <c r="C197" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198">
-        <v>1901</v>
+        <v>1702</v>
       </c>
       <c r="B198" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="C198" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199">
+        <v>1703</v>
+      </c>
+      <c r="B199" t="s">
+        <v>104</v>
+      </c>
+      <c r="C199" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
+      <c r="A200">
+        <v>1704</v>
+      </c>
+      <c r="B200" t="s">
+        <v>126</v>
+      </c>
+      <c r="C200" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201">
-        <v>2001</v>
+        <v>1705</v>
       </c>
       <c r="B201" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C201" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202">
-        <v>2002</v>
+        <v>1706</v>
       </c>
       <c r="B202" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C202" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203">
-        <v>2003</v>
+        <v>1707</v>
       </c>
       <c r="B203" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C203" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204">
-        <v>2004</v>
+        <v>1708</v>
       </c>
       <c r="B204" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C204" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="A205">
-        <v>2005</v>
-      </c>
-      <c r="B205" t="s">
-        <v>156</v>
-      </c>
-      <c r="C205" t="s">
-        <v>151</v>
-      </c>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
     </row>
     <row r="207" spans="1:3">
-      <c r="A207" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
+      <c r="A207">
+        <v>1801</v>
+      </c>
+      <c r="B207" t="s">
+        <v>146</v>
+      </c>
+      <c r="C207" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208">
-        <v>2101</v>
+        <v>1802</v>
       </c>
       <c r="B208" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C208" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209">
-        <v>2102</v>
-      </c>
-      <c r="B209" t="s">
-        <v>153</v>
-      </c>
-      <c r="C209" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210">
-        <v>2103</v>
-      </c>
-      <c r="B210" t="s">
-        <v>165</v>
-      </c>
-      <c r="C210" t="s">
-        <v>164</v>
-      </c>
+      <c r="A210" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
+        <v>1901</v>
+      </c>
+      <c r="B211" t="s">
+        <v>149</v>
+      </c>
+      <c r="C211" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214">
+        <v>2001</v>
+      </c>
+      <c r="B214" t="s">
+        <v>151</v>
+      </c>
+      <c r="C214" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215">
+        <v>2002</v>
+      </c>
+      <c r="B215" t="s">
+        <v>152</v>
+      </c>
+      <c r="C215" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216">
+        <v>2003</v>
+      </c>
+      <c r="B216" t="s">
+        <v>153</v>
+      </c>
+      <c r="C216" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217">
+        <v>2004</v>
+      </c>
+      <c r="B217" t="s">
+        <v>154</v>
+      </c>
+      <c r="C217" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218">
+        <v>2005</v>
+      </c>
+      <c r="B218" t="s">
+        <v>155</v>
+      </c>
+      <c r="C218" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221">
+        <v>2101</v>
+      </c>
+      <c r="B221" t="s">
+        <v>151</v>
+      </c>
+      <c r="C221" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222">
+        <v>2102</v>
+      </c>
+      <c r="B222" t="s">
+        <v>152</v>
+      </c>
+      <c r="C222" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223">
+        <v>2103</v>
+      </c>
+      <c r="B223" t="s">
+        <v>164</v>
+      </c>
+      <c r="C223" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224">
         <v>2104</v>
       </c>
-      <c r="B211" t="s">
-        <v>167</v>
-      </c>
-      <c r="C211" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="A212">
+      <c r="B224" t="s">
+        <v>166</v>
+      </c>
+      <c r="C224" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225">
         <v>2105</v>
       </c>
-      <c r="B212" t="s">
-        <v>166</v>
-      </c>
-      <c r="C212" t="s">
-        <v>164</v>
+      <c r="B225" t="s">
+        <v>165</v>
+      </c>
+      <c r="C225" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A207:C207"/>
-    <mergeCell ref="A193:C193"/>
-    <mergeCell ref="A197:C197"/>
-    <mergeCell ref="A200:C200"/>
-    <mergeCell ref="A176:C176"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A162:C162"/>
+    <mergeCell ref="A220:C220"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A210:C210"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A180:C180"/>
+    <mergeCell ref="A196:C196"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-18#8 ## Update database server (production).    - Add TABLE/VIEW/SP for Error message (supports ML).    - Generate and Update all db scripts until 2018-05-18 (today).    - Update server update history.    - Update project history.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="195">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -589,6 +589,18 @@
   </si>
   <si>
     <t>Question Item Text (ML) already exists.</t>
+  </si>
+  <si>
+    <t>ErrorMessages</t>
+  </si>
+  <si>
+    <t>SaveErrorMsgML</t>
+  </si>
+  <si>
+    <t>Error Code cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Error Message (ML) cannot be null or empty string.</t>
   </si>
 </sst>
 </file>
@@ -932,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3286,29 +3298,81 @@
         <v>163</v>
       </c>
     </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235">
+        <v>2201</v>
+      </c>
+      <c r="B235" t="s">
+        <v>193</v>
+      </c>
+      <c r="C235" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236">
+        <v>2202</v>
+      </c>
+      <c r="B236" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237">
+        <v>2203</v>
+      </c>
+      <c r="B237" t="s">
+        <v>21</v>
+      </c>
+      <c r="C237" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238">
+        <v>2204</v>
+      </c>
+      <c r="B238" t="s">
+        <v>194</v>
+      </c>
+      <c r="C238" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A162:C162"/>
+  <mergeCells count="22">
+    <mergeCell ref="A234:C234"/>
     <mergeCell ref="A227:C227"/>
     <mergeCell ref="A213:C213"/>
     <mergeCell ref="A217:C217"/>
     <mergeCell ref="A220:C220"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A203:C203"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A162:C162"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-22#1 ## Clean up projects.    - move all code to v1.    - Remove all code to rewrite.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="200">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -601,6 +601,21 @@
   </si>
   <si>
     <t>Error Message (ML) cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>RegisterClient</t>
+  </si>
+  <si>
+    <t>Client Id cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Client is already registered.</t>
+  </si>
+  <si>
+    <t>Client Init Date cannot be null.</t>
   </si>
 </sst>
 </file>
@@ -944,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C238"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3349,13 +3364,59 @@
         <v>192</v>
       </c>
     </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B240" s="2"/>
+      <c r="C240" s="2"/>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241">
+        <v>2301</v>
+      </c>
+      <c r="B241" t="s">
+        <v>197</v>
+      </c>
+      <c r="C241" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242">
+        <v>2302</v>
+      </c>
+      <c r="B242" t="s">
+        <v>199</v>
+      </c>
+      <c r="C242" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243">
+        <v>2303</v>
+      </c>
+      <c r="B243" t="s">
+        <v>198</v>
+      </c>
+      <c r="C243" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A234:C234"/>
-    <mergeCell ref="A227:C227"/>
-    <mergeCell ref="A213:C213"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A220:C220"/>
+  <mergeCells count="23">
+    <mergeCell ref="A240:C240"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A88:C88"/>
     <mergeCell ref="A180:C180"/>
     <mergeCell ref="A203:C203"/>
     <mergeCell ref="A99:C99"/>
@@ -3363,16 +3424,11 @@
     <mergeCell ref="A134:C134"/>
     <mergeCell ref="A142:C142"/>
     <mergeCell ref="A162:C162"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A234:C234"/>
+    <mergeCell ref="A227:C227"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A217:C217"/>
+    <mergeCell ref="A220:C220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-24#7 ## Update api routes    - setup api routes part 5
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="208">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -616,6 +616,30 @@
   </si>
   <si>
     <t>Client Init Date cannot be null.</t>
+  </si>
+  <si>
+    <t>Device Type Id not found.</t>
+  </si>
+  <si>
+    <t>Device Name (default) cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Device Id is not found.</t>
+  </si>
+  <si>
+    <t>Device Name (default) already exists.</t>
+  </si>
+  <si>
+    <t>SaveDevice</t>
+  </si>
+  <si>
+    <t>SaveDeviceML</t>
+  </si>
+  <si>
+    <t>Device Id cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Device Name (ML) is already exists.</t>
   </si>
 </sst>
 </file>
@@ -959,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C243"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="A258" sqref="A258:XFD260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3404,8 +3428,155 @@
         <v>196</v>
       </c>
     </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246">
+        <v>2401</v>
+      </c>
+      <c r="B246" t="s">
+        <v>90</v>
+      </c>
+      <c r="C246" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247">
+        <v>2402</v>
+      </c>
+      <c r="B247" t="s">
+        <v>200</v>
+      </c>
+      <c r="C247" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248">
+        <v>2403</v>
+      </c>
+      <c r="B248" t="s">
+        <v>201</v>
+      </c>
+      <c r="C248" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249">
+        <v>2404</v>
+      </c>
+      <c r="B249" t="s">
+        <v>97</v>
+      </c>
+      <c r="C249" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250">
+        <v>2405</v>
+      </c>
+      <c r="B250" t="s">
+        <v>202</v>
+      </c>
+      <c r="C250" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251">
+        <v>2406</v>
+      </c>
+      <c r="B251" t="s">
+        <v>203</v>
+      </c>
+      <c r="C251" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252">
+        <v>2407</v>
+      </c>
+      <c r="B252" t="s">
+        <v>90</v>
+      </c>
+      <c r="C252" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253">
+        <v>2408</v>
+      </c>
+      <c r="B253" t="s">
+        <v>86</v>
+      </c>
+      <c r="C253" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254">
+        <v>2409</v>
+      </c>
+      <c r="B254" t="s">
+        <v>120</v>
+      </c>
+      <c r="C254" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255">
+        <v>2410</v>
+      </c>
+      <c r="B255" t="s">
+        <v>206</v>
+      </c>
+      <c r="C255" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256">
+        <v>2411</v>
+      </c>
+      <c r="B256" t="s">
+        <v>202</v>
+      </c>
+      <c r="C256" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257">
+        <v>2412</v>
+      </c>
+      <c r="B257" t="s">
+        <v>207</v>
+      </c>
+      <c r="C257" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A162:C162"/>
+    <mergeCell ref="A234:C234"/>
+    <mergeCell ref="A227:C227"/>
+    <mergeCell ref="A213:C213"/>
+    <mergeCell ref="A217:C217"/>
+    <mergeCell ref="A220:C220"/>
     <mergeCell ref="A240:C240"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A3:C3"/>
@@ -3422,13 +3593,6 @@
     <mergeCell ref="A99:C99"/>
     <mergeCell ref="A118:C118"/>
     <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A162:C162"/>
-    <mergeCell ref="A234:C234"/>
-    <mergeCell ref="A227:C227"/>
-    <mergeCell ref="A213:C213"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A220:C220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-24#13 ## Update db scripts.    # TABLES and VIEWS      - Add LogInView (VIEW). ## SPs    - Add SignIn (Customer) SP. ## Update db definition.    - Update wrapper code for SignIn SP. ## Update api routes    - setup SignIn api route.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="209">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -465,9 +465,6 @@
     <t>SignIn</t>
   </si>
   <si>
-    <t>Reserved not exist.</t>
-  </si>
-  <si>
     <t>GetVoteSummaries</t>
   </si>
   <si>
@@ -640,6 +637,12 @@
   </si>
   <si>
     <t>Device Name (ML) is already exists.</t>
+  </si>
+  <si>
+    <t>Cannot found User that match information.</t>
+  </si>
+  <si>
+    <t>Register</t>
   </si>
 </sst>
 </file>
@@ -983,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C257"/>
+  <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258:XFD260"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="A259" sqref="A259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2411,1058 +2414,1098 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-    </row>
     <row r="135" spans="1:3">
-      <c r="A135">
-        <v>1301</v>
-      </c>
+      <c r="A135" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>1302</v>
+        <v>1401</v>
+      </c>
+      <c r="B136" t="s">
+        <v>90</v>
+      </c>
+      <c r="C136" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137">
-        <v>1303</v>
+        <v>1402</v>
+      </c>
+      <c r="B137" t="s">
+        <v>97</v>
+      </c>
+      <c r="C137" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>1304</v>
+        <v>1403</v>
+      </c>
+      <c r="B138" t="s">
+        <v>156</v>
+      </c>
+      <c r="C138" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>1305</v>
+        <v>1404</v>
+      </c>
+      <c r="B139" t="s">
+        <v>157</v>
+      </c>
+      <c r="C139" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>1306</v>
+        <v>1405</v>
+      </c>
+      <c r="B140" t="s">
+        <v>158</v>
+      </c>
+      <c r="C140" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>1406</v>
+      </c>
+      <c r="B141" t="s">
+        <v>159</v>
+      </c>
+      <c r="C141" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
+      <c r="A142">
+        <v>1407</v>
+      </c>
+      <c r="B142" t="s">
+        <v>160</v>
+      </c>
+      <c r="C142" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143">
-        <v>1401</v>
+        <v>1408</v>
       </c>
       <c r="B143" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="C143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
-        <v>1402</v>
+        <v>1409</v>
       </c>
       <c r="B144" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C144" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145">
-        <v>1403</v>
+        <v>1410</v>
       </c>
       <c r="B145" t="s">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="C145" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146">
-        <v>1404</v>
+        <v>1411</v>
       </c>
       <c r="B146" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
       <c r="C146" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147">
-        <v>1405</v>
+        <v>1412</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="C147" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148">
-        <v>1406</v>
+        <v>1413</v>
       </c>
       <c r="B148" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C148" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149">
-        <v>1407</v>
+        <v>1414</v>
       </c>
       <c r="B149" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C149" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150">
-        <v>1408</v>
+        <v>1415</v>
       </c>
       <c r="B150" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C150" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151">
-        <v>1409</v>
+        <v>1416</v>
       </c>
       <c r="B151" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="C151" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152">
-        <v>1410</v>
+        <v>1417</v>
       </c>
       <c r="B152" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="C152" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153">
-        <v>1411</v>
+        <v>1418</v>
       </c>
       <c r="B153" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="C153" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154">
-        <v>1412</v>
-      </c>
-      <c r="B154" t="s">
-        <v>108</v>
-      </c>
-      <c r="C154" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155">
-        <v>1413</v>
-      </c>
-      <c r="B155" t="s">
-        <v>152</v>
-      </c>
-      <c r="C155" t="s">
-        <v>167</v>
-      </c>
+      <c r="A155" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
     </row>
     <row r="156" spans="1:3">
       <c r="A156">
-        <v>1414</v>
+        <v>1501</v>
       </c>
       <c r="B156" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="C156" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157">
-        <v>1415</v>
+        <v>1502</v>
       </c>
       <c r="B157" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C157" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158">
-        <v>1416</v>
+        <v>1503</v>
       </c>
       <c r="B158" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="C158" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159">
-        <v>1417</v>
+        <v>1504</v>
       </c>
       <c r="B159" t="s">
+        <v>97</v>
+      </c>
+      <c r="C159" t="s">
         <v>170</v>
-      </c>
-      <c r="C159" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160">
-        <v>1418</v>
+        <v>1505</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>173</v>
       </c>
       <c r="C160" t="s">
-        <v>167</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>1506</v>
+      </c>
+      <c r="B161" t="s">
+        <v>174</v>
+      </c>
+      <c r="C161" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
+      <c r="A162">
+        <v>1507</v>
+      </c>
+      <c r="B162" t="s">
+        <v>86</v>
+      </c>
+      <c r="C162" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>1501</v>
+        <v>1508</v>
       </c>
       <c r="B163" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C163" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>1502</v>
+        <v>1509</v>
       </c>
       <c r="B164" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="C164" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165">
-        <v>1503</v>
+        <v>1510</v>
       </c>
       <c r="B165" t="s">
-        <v>173</v>
+        <v>108</v>
       </c>
       <c r="C165" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>1504</v>
+        <v>1511</v>
       </c>
       <c r="B166" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="C166" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167">
-        <v>1505</v>
+        <v>1512</v>
       </c>
       <c r="B167" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C167" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168">
-        <v>1506</v>
+        <v>1513</v>
       </c>
       <c r="B168" t="s">
+        <v>176</v>
+      </c>
+      <c r="C168" t="s">
         <v>175</v>
-      </c>
-      <c r="C168" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>1507</v>
+        <v>1514</v>
       </c>
       <c r="B169" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="C169" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>1508</v>
+        <v>1515</v>
       </c>
       <c r="B170" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="C170" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>1509</v>
+        <v>1516</v>
       </c>
       <c r="B171" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="C171" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172">
-        <v>1510</v>
-      </c>
-      <c r="B172" t="s">
-        <v>108</v>
-      </c>
-      <c r="C172" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173">
-        <v>1511</v>
-      </c>
-      <c r="B173" t="s">
-        <v>152</v>
-      </c>
-      <c r="C173" t="s">
-        <v>176</v>
-      </c>
+      <c r="A173" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
-        <v>1512</v>
+        <v>1601</v>
       </c>
       <c r="B174" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="C174" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175">
-        <v>1513</v>
+        <v>1602</v>
       </c>
       <c r="B175" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C175" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176">
-        <v>1514</v>
+        <v>1603</v>
       </c>
       <c r="B176" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C176" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>1515</v>
+        <v>1604</v>
       </c>
       <c r="B177" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C177" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>1516</v>
+        <v>1605</v>
       </c>
       <c r="B178" t="s">
-        <v>180</v>
+        <v>97</v>
       </c>
       <c r="C178" t="s">
-        <v>176</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179">
+        <v>1606</v>
+      </c>
+      <c r="B179" t="s">
+        <v>173</v>
+      </c>
+      <c r="C179" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="2" t="s">
+      <c r="A180">
+        <v>1607</v>
+      </c>
+      <c r="B180" t="s">
+        <v>183</v>
+      </c>
+      <c r="C180" t="s">
         <v>181</v>
       </c>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>1601</v>
+        <v>1608</v>
       </c>
       <c r="B181" t="s">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="C181" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182">
-        <v>1602</v>
+        <v>1609</v>
       </c>
       <c r="B182" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="C182" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183">
-        <v>1603</v>
+        <v>1610</v>
       </c>
       <c r="B183" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="C183" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>1604</v>
+        <v>1611</v>
       </c>
       <c r="B184" t="s">
-        <v>173</v>
+        <v>90</v>
       </c>
       <c r="C184" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185">
-        <v>1605</v>
+        <v>1612</v>
       </c>
       <c r="B185" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C185" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>1606</v>
+        <v>1613</v>
       </c>
       <c r="B186" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C186" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>1607</v>
+        <v>1614</v>
       </c>
       <c r="B187" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C187" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>1608</v>
+        <v>1615</v>
       </c>
       <c r="B188" t="s">
+        <v>176</v>
+      </c>
+      <c r="C188" t="s">
         <v>185</v>
-      </c>
-      <c r="C188" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>1609</v>
+        <v>1616</v>
       </c>
       <c r="B189" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="C189" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>1610</v>
+        <v>1617</v>
       </c>
       <c r="B190" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="C190" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191">
-        <v>1611</v>
+        <v>1618</v>
       </c>
       <c r="B191" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="C191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192">
-        <v>1612</v>
+        <v>1619</v>
       </c>
       <c r="B192" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="C192" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193">
-        <v>1613</v>
+        <v>1620</v>
       </c>
       <c r="B193" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="C193" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194">
-        <v>1614</v>
-      </c>
-      <c r="B194" t="s">
-        <v>168</v>
+        <v>1621</v>
       </c>
       <c r="C194" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195">
-        <v>1615</v>
-      </c>
-      <c r="B195" t="s">
-        <v>177</v>
-      </c>
-      <c r="C195" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196">
-        <v>1616</v>
-      </c>
-      <c r="B196" t="s">
-        <v>178</v>
-      </c>
-      <c r="C196" t="s">
-        <v>186</v>
-      </c>
+      <c r="A196" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
     </row>
     <row r="197" spans="1:3">
       <c r="A197">
-        <v>1617</v>
+        <v>1701</v>
       </c>
       <c r="B197" t="s">
-        <v>187</v>
+        <v>90</v>
       </c>
       <c r="C197" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198">
-        <v>1618</v>
+        <v>1702</v>
       </c>
       <c r="B198" t="s">
-        <v>188</v>
+        <v>108</v>
       </c>
       <c r="C198" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199">
-        <v>1619</v>
+        <v>1703</v>
       </c>
       <c r="B199" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="C199" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200">
-        <v>1620</v>
+        <v>1704</v>
       </c>
       <c r="B200" t="s">
-        <v>190</v>
+        <v>126</v>
       </c>
       <c r="C200" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201">
-        <v>1621</v>
+        <v>1705</v>
+      </c>
+      <c r="B201" t="s">
+        <v>132</v>
       </c>
       <c r="C201" t="s">
-        <v>186</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202">
+        <v>1706</v>
+      </c>
+      <c r="B202" t="s">
+        <v>139</v>
+      </c>
+      <c r="C202" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
+      <c r="A203">
+        <v>1707</v>
+      </c>
+      <c r="B203" t="s">
+        <v>141</v>
+      </c>
+      <c r="C203" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204">
-        <v>1701</v>
+        <v>1708</v>
       </c>
       <c r="B204" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="C204" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
-      <c r="A205">
-        <v>1702</v>
-      </c>
-      <c r="B205" t="s">
-        <v>108</v>
-      </c>
-      <c r="C205" t="s">
-        <v>140</v>
-      </c>
-    </row>
     <row r="206" spans="1:3">
-      <c r="A206">
-        <v>1703</v>
-      </c>
-      <c r="B206" t="s">
-        <v>104</v>
-      </c>
-      <c r="C206" t="s">
-        <v>140</v>
-      </c>
+      <c r="A206" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
     </row>
     <row r="207" spans="1:3">
       <c r="A207">
-        <v>1704</v>
+        <v>1801</v>
       </c>
       <c r="B207" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C207" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208">
-        <v>1705</v>
+        <v>1802</v>
       </c>
       <c r="B208" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C208" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209">
-        <v>1706</v>
-      </c>
-      <c r="B209" t="s">
-        <v>139</v>
-      </c>
-      <c r="C209" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210">
-        <v>1707</v>
-      </c>
-      <c r="B210" t="s">
-        <v>141</v>
-      </c>
-      <c r="C210" t="s">
-        <v>140</v>
-      </c>
+      <c r="A210" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
-        <v>1708</v>
+        <v>1901</v>
       </c>
       <c r="B211" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="C211" t="s">
-        <v>140</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212">
+        <v>1902</v>
+      </c>
+      <c r="B212" t="s">
+        <v>109</v>
+      </c>
+      <c r="C212" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
+      <c r="A213">
+        <v>1903</v>
+      </c>
+      <c r="B213" t="s">
+        <v>41</v>
+      </c>
+      <c r="C213" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214">
-        <v>1801</v>
+        <v>1904</v>
       </c>
       <c r="B214" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="C214" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
-      <c r="A215">
-        <v>1802</v>
-      </c>
-      <c r="B215" t="s">
-        <v>147</v>
-      </c>
-      <c r="C215" t="s">
-        <v>145</v>
-      </c>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
+      <c r="A217">
+        <v>2001</v>
+      </c>
+      <c r="B217" t="s">
+        <v>150</v>
+      </c>
+      <c r="C217" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>1901</v>
+        <v>2002</v>
       </c>
       <c r="B218" t="s">
+        <v>151</v>
+      </c>
+      <c r="C218" t="s">
         <v>149</v>
       </c>
-      <c r="C218" t="s">
-        <v>148</v>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219">
+        <v>2003</v>
+      </c>
+      <c r="B219" t="s">
+        <v>152</v>
+      </c>
+      <c r="C219" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
+      <c r="A220">
+        <v>2004</v>
+      </c>
+      <c r="B220" t="s">
+        <v>153</v>
+      </c>
+      <c r="C220" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="B221" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C221" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222">
-        <v>2002</v>
-      </c>
-      <c r="B222" t="s">
-        <v>152</v>
-      </c>
-      <c r="C222" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223">
-        <v>2003</v>
-      </c>
-      <c r="B223" t="s">
-        <v>153</v>
-      </c>
-      <c r="C223" t="s">
-        <v>150</v>
-      </c>
+      <c r="A223" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>2004</v>
+        <v>2101</v>
       </c>
       <c r="B224" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C224" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225">
-        <v>2005</v>
+        <v>2102</v>
       </c>
       <c r="B225" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C225" t="s">
-        <v>150</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226">
+        <v>2103</v>
+      </c>
+      <c r="B226" t="s">
+        <v>163</v>
+      </c>
+      <c r="C226" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
+      <c r="A227">
+        <v>2104</v>
+      </c>
+      <c r="B227" t="s">
+        <v>165</v>
+      </c>
+      <c r="C227" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228">
-        <v>2101</v>
+        <v>2105</v>
       </c>
       <c r="B228" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C228" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229">
-        <v>2102</v>
-      </c>
-      <c r="B229" t="s">
-        <v>152</v>
-      </c>
-      <c r="C229" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="230" spans="1:3">
-      <c r="A230">
-        <v>2103</v>
-      </c>
-      <c r="B230" t="s">
-        <v>164</v>
-      </c>
-      <c r="C230" t="s">
-        <v>163</v>
-      </c>
+      <c r="A230" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B230" s="2"/>
+      <c r="C230" s="2"/>
     </row>
     <row r="231" spans="1:3">
       <c r="A231">
-        <v>2104</v>
+        <v>2201</v>
       </c>
       <c r="B231" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C231" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232">
-        <v>2105</v>
+        <v>2202</v>
       </c>
       <c r="B232" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
       <c r="C232" t="s">
-        <v>163</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233">
+        <v>2203</v>
+      </c>
+      <c r="B233" t="s">
+        <v>21</v>
+      </c>
+      <c r="C233" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="234" spans="1:3">
-      <c r="A234" s="2" t="s">
+      <c r="A234">
+        <v>2204</v>
+      </c>
+      <c r="B234" t="s">
+        <v>193</v>
+      </c>
+      <c r="C234" t="s">
         <v>191</v>
       </c>
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235">
-        <v>2201</v>
-      </c>
-      <c r="B235" t="s">
-        <v>193</v>
-      </c>
-      <c r="C235" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="236" spans="1:3">
-      <c r="A236">
-        <v>2202</v>
-      </c>
-      <c r="B236" t="s">
-        <v>6</v>
-      </c>
-      <c r="C236" t="s">
-        <v>192</v>
-      </c>
+      <c r="A236" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
     </row>
     <row r="237" spans="1:3">
       <c r="A237">
-        <v>2203</v>
+        <v>2301</v>
       </c>
       <c r="B237" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="C237" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238">
-        <v>2204</v>
+        <v>2302</v>
       </c>
       <c r="B238" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C238" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239">
+        <v>2303</v>
+      </c>
+      <c r="B239" t="s">
+        <v>197</v>
+      </c>
+      <c r="C239" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="241" spans="1:3">
-      <c r="A241">
-        <v>2301</v>
-      </c>
-      <c r="B241" t="s">
-        <v>197</v>
-      </c>
-      <c r="C241" t="s">
-        <v>196</v>
-      </c>
+      <c r="A241" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
     </row>
     <row r="242" spans="1:3">
       <c r="A242">
-        <v>2302</v>
+        <v>2401</v>
       </c>
       <c r="B242" t="s">
-        <v>199</v>
+        <v>90</v>
       </c>
       <c r="C242" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243">
-        <v>2303</v>
+        <v>2402</v>
       </c>
       <c r="B243" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C243" t="s">
-        <v>196</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244">
+        <v>2403</v>
+      </c>
+      <c r="B244" t="s">
+        <v>200</v>
+      </c>
+      <c r="C244" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
+      <c r="A245">
+        <v>2404</v>
+      </c>
+      <c r="B245" t="s">
+        <v>97</v>
+      </c>
+      <c r="C245" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246">
-        <v>2401</v>
+        <v>2405</v>
       </c>
       <c r="B246" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="C246" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247">
-        <v>2402</v>
+        <v>2406</v>
       </c>
       <c r="B247" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C247" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248">
-        <v>2403</v>
+        <v>2407</v>
       </c>
       <c r="B248" t="s">
-        <v>201</v>
+        <v>90</v>
       </c>
       <c r="C248" t="s">
         <v>204</v>
@@ -3470,10 +3513,10 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249">
-        <v>2404</v>
+        <v>2408</v>
       </c>
       <c r="B249" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C249" t="s">
         <v>204</v>
@@ -3481,10 +3524,10 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250">
-        <v>2405</v>
+        <v>2409</v>
       </c>
       <c r="B250" t="s">
-        <v>202</v>
+        <v>120</v>
       </c>
       <c r="C250" t="s">
         <v>204</v>
@@ -3492,10 +3535,10 @@
     </row>
     <row r="251" spans="1:3">
       <c r="A251">
-        <v>2406</v>
+        <v>2410</v>
       </c>
       <c r="B251" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C251" t="s">
         <v>204</v>
@@ -3503,96 +3546,51 @@
     </row>
     <row r="252" spans="1:3">
       <c r="A252">
-        <v>2407</v>
+        <v>2411</v>
       </c>
       <c r="B252" t="s">
-        <v>90</v>
+        <v>201</v>
       </c>
       <c r="C252" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253">
-        <v>2408</v>
+        <v>2412</v>
       </c>
       <c r="B253" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="C253" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254">
-        <v>2409</v>
-      </c>
-      <c r="B254" t="s">
-        <v>120</v>
-      </c>
-      <c r="C254" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255">
-        <v>2410</v>
-      </c>
-      <c r="B255" t="s">
-        <v>206</v>
-      </c>
-      <c r="C255" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
-      <c r="A256">
-        <v>2411</v>
-      </c>
-      <c r="B256" t="s">
-        <v>202</v>
-      </c>
-      <c r="C256" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="A257">
-        <v>2412</v>
-      </c>
-      <c r="B257" t="s">
-        <v>207</v>
-      </c>
-      <c r="C257" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A162:C162"/>
-    <mergeCell ref="A234:C234"/>
-    <mergeCell ref="A227:C227"/>
-    <mergeCell ref="A213:C213"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A220:C220"/>
-    <mergeCell ref="A240:C240"/>
+  <mergeCells count="23">
+    <mergeCell ref="A241:C241"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A155:C155"/>
+    <mergeCell ref="A230:C230"/>
+    <mergeCell ref="A223:C223"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A210:C210"/>
+    <mergeCell ref="A216:C216"/>
+    <mergeCell ref="A236:C236"/>
+    <mergeCell ref="A173:C173"/>
+    <mergeCell ref="A196:C196"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A180:C180"/>
-    <mergeCell ref="A203:C203"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A134:C134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-25#4 ## Database script update.    - Add ClientAccess Table.    - Update SignIn SP.    - Add CheckAccess SP. ## Server Code Update.    - Add definition file for CheckAccess SP.    - Add wrapper code for CheckAccess SP.    - Add route for CheckAccess SP.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="208">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -603,18 +603,6 @@
     <t>Clients</t>
   </si>
   <si>
-    <t>RegisterClient</t>
-  </si>
-  <si>
-    <t>Client Id cannot be null or empty string.</t>
-  </si>
-  <si>
-    <t>Client is already registered.</t>
-  </si>
-  <si>
-    <t>Client Init Date cannot be null.</t>
-  </si>
-  <si>
     <t>Device Type Id not found.</t>
   </si>
   <si>
@@ -643,6 +631,15 @@
   </si>
   <si>
     <t>Register</t>
+  </si>
+  <si>
+    <t>CheckAccess</t>
+  </si>
+  <si>
+    <t>Access Id cannot be null or empty string.</t>
+  </si>
+  <si>
+    <t>Access Id not found.</t>
   </si>
 </sst>
 </file>
@@ -988,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="A259" sqref="A259"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3134,7 +3131,7 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -3173,7 +3170,7 @@
         <v>1901</v>
       </c>
       <c r="B211" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C211" t="s">
         <v>148</v>
@@ -3184,7 +3181,7 @@
         <v>1902</v>
       </c>
       <c r="B212" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="C212" t="s">
         <v>148</v>
@@ -3195,7 +3192,7 @@
         <v>1903</v>
       </c>
       <c r="B213" t="s">
-        <v>41</v>
+        <v>203</v>
       </c>
       <c r="C213" t="s">
         <v>148</v>
@@ -3205,9 +3202,6 @@
       <c r="A214">
         <v>1904</v>
       </c>
-      <c r="B214" t="s">
-        <v>207</v>
-      </c>
       <c r="C214" t="s">
         <v>148</v>
       </c>
@@ -3399,10 +3393,10 @@
         <v>2301</v>
       </c>
       <c r="B237" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C237" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3410,21 +3404,18 @@
         <v>2302</v>
       </c>
       <c r="B238" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C238" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239">
         <v>2303</v>
       </c>
-      <c r="B239" t="s">
-        <v>197</v>
-      </c>
       <c r="C239" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3442,7 +3433,7 @@
         <v>90</v>
       </c>
       <c r="C242" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3450,10 +3441,10 @@
         <v>2402</v>
       </c>
       <c r="B243" t="s">
+        <v>195</v>
+      </c>
+      <c r="C243" t="s">
         <v>199</v>
-      </c>
-      <c r="C243" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3461,10 +3452,10 @@
         <v>2403</v>
       </c>
       <c r="B244" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C244" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3475,7 +3466,7 @@
         <v>97</v>
       </c>
       <c r="C245" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3483,10 +3474,10 @@
         <v>2405</v>
       </c>
       <c r="B246" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C246" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3494,10 +3485,10 @@
         <v>2406</v>
       </c>
       <c r="B247" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C247" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3508,7 +3499,7 @@
         <v>90</v>
       </c>
       <c r="C248" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3519,7 +3510,7 @@
         <v>86</v>
       </c>
       <c r="C249" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3530,7 +3521,7 @@
         <v>120</v>
       </c>
       <c r="C250" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3538,10 +3529,10 @@
         <v>2410</v>
       </c>
       <c r="B251" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C251" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3549,10 +3540,10 @@
         <v>2411</v>
       </c>
       <c r="B252" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C252" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3560,14 +3551,26 @@
         <v>2412</v>
       </c>
       <c r="B253" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C253" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A241:C241"/>
     <mergeCell ref="A135:C135"/>
     <mergeCell ref="A155:C155"/>
@@ -3579,18 +3582,6 @@
     <mergeCell ref="A236:C236"/>
     <mergeCell ref="A173:C173"/>
     <mergeCell ref="A196:C196"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A88:C88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 2018-05-25#5 ## Database script update.    - Update SignIn SP.    - Update CheckAccess SP.    - Add GetCurrentUser SP.    - Add SignOut SP. ## Server Code Update.    - Add definition file for GetCurrentUser SP.    - Add wrapper code for GetCurrentUser SP.    - Add route for GetCurrentUser SP.    - Add definition file for SignOut SP.    - Add wrapper code for SignOut SP.    - Add route for SignOut SP.
</commit_message>
<xml_diff>
--- a/db/db.error.code.xlsx
+++ b/db/db.error.code.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="210">
   <si>
     <t>ErrorCode</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>Access Id not found.</t>
+  </si>
+  <si>
+    <t>GetAccessUser</t>
+  </si>
+  <si>
+    <t>SignOut</t>
   </si>
 </sst>
 </file>
@@ -983,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+      <selection activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3198,27 +3204,30 @@
         <v>148</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
-      <c r="A214">
-        <v>1904</v>
-      </c>
-      <c r="C214" t="s">
-        <v>148</v>
-      </c>
+    <row r="215" spans="1:3">
+      <c r="A215" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
     </row>
     <row r="216" spans="1:3">
-      <c r="A216" s="2" t="s">
+      <c r="A216">
+        <v>2001</v>
+      </c>
+      <c r="B216" t="s">
+        <v>150</v>
+      </c>
+      <c r="C216" t="s">
         <v>149</v>
       </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
     </row>
     <row r="217" spans="1:3">
       <c r="A217">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B217" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C217" t="s">
         <v>149</v>
@@ -3226,10 +3235,10 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B218" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C218" t="s">
         <v>149</v>
@@ -3237,10 +3246,10 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B219" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C219" t="s">
         <v>149</v>
@@ -3248,39 +3257,39 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B220" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C220" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
-      <c r="A221">
-        <v>2005</v>
-      </c>
-      <c r="B221" t="s">
-        <v>154</v>
-      </c>
-      <c r="C221" t="s">
-        <v>149</v>
-      </c>
+    <row r="222" spans="1:3">
+      <c r="A222" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="2" t="s">
+      <c r="A223">
+        <v>2101</v>
+      </c>
+      <c r="B223" t="s">
+        <v>150</v>
+      </c>
+      <c r="C223" t="s">
         <v>162</v>
       </c>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>2101</v>
+        <v>2102</v>
       </c>
       <c r="B224" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C224" t="s">
         <v>162</v>
@@ -3288,10 +3297,10 @@
     </row>
     <row r="225" spans="1:3">
       <c r="A225">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="B225" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C225" t="s">
         <v>162</v>
@@ -3299,10 +3308,10 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226">
-        <v>2103</v>
+        <v>2104</v>
       </c>
       <c r="B226" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C226" t="s">
         <v>162</v>
@@ -3310,39 +3319,39 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227">
-        <v>2104</v>
+        <v>2105</v>
       </c>
       <c r="B227" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C227" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
-      <c r="A228">
-        <v>2105</v>
-      </c>
-      <c r="B228" t="s">
-        <v>164</v>
-      </c>
-      <c r="C228" t="s">
-        <v>162</v>
-      </c>
+    <row r="229" spans="1:3">
+      <c r="A229" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
     </row>
     <row r="230" spans="1:3">
-      <c r="A230" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
+      <c r="A230">
+        <v>2201</v>
+      </c>
+      <c r="B230" t="s">
+        <v>192</v>
+      </c>
+      <c r="C230" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="B231" t="s">
-        <v>192</v>
+        <v>6</v>
       </c>
       <c r="C231" t="s">
         <v>191</v>
@@ -3350,10 +3359,10 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="B232" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C232" t="s">
         <v>191</v>
@@ -3361,39 +3370,39 @@
     </row>
     <row r="233" spans="1:3">
       <c r="A233">
-        <v>2203</v>
+        <v>2204</v>
       </c>
       <c r="B233" t="s">
-        <v>21</v>
+        <v>193</v>
       </c>
       <c r="C233" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
-      <c r="A234">
-        <v>2204</v>
-      </c>
-      <c r="B234" t="s">
-        <v>193</v>
-      </c>
-      <c r="C234" t="s">
-        <v>191</v>
-      </c>
+    <row r="235" spans="1:3">
+      <c r="A235" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
     </row>
     <row r="236" spans="1:3">
-      <c r="A236" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B236" s="2"/>
-      <c r="C236" s="2"/>
+      <c r="A236">
+        <v>2301</v>
+      </c>
+      <c r="B236" t="s">
+        <v>206</v>
+      </c>
+      <c r="C236" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237">
-        <v>2301</v>
+        <v>2302</v>
       </c>
       <c r="B237" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C237" t="s">
         <v>205</v>
@@ -3401,80 +3410,83 @@
     </row>
     <row r="238" spans="1:3">
       <c r="A238">
-        <v>2302</v>
+        <v>2303</v>
       </c>
       <c r="B238" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="C238" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239">
-        <v>2303</v>
+        <v>2304</v>
+      </c>
+      <c r="B239" t="s">
+        <v>89</v>
       </c>
       <c r="C239" t="s">
-        <v>205</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240">
+        <v>2305</v>
+      </c>
+      <c r="B240" t="s">
+        <v>206</v>
+      </c>
+      <c r="C240" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="241" spans="1:3">
-      <c r="A241" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
+      <c r="A241">
+        <v>2306</v>
+      </c>
+      <c r="B241" t="s">
+        <v>207</v>
+      </c>
+      <c r="C241" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242">
-        <v>2401</v>
+        <v>2307</v>
       </c>
       <c r="B242" t="s">
-        <v>90</v>
+        <v>206</v>
       </c>
       <c r="C242" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243">
-        <v>2402</v>
+        <v>2308</v>
       </c>
       <c r="B243" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C243" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244">
-        <v>2403</v>
-      </c>
-      <c r="B244" t="s">
-        <v>196</v>
-      </c>
-      <c r="C244" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="245" spans="1:3">
-      <c r="A245">
-        <v>2404</v>
-      </c>
-      <c r="B245" t="s">
-        <v>97</v>
-      </c>
-      <c r="C245" t="s">
-        <v>199</v>
-      </c>
+      <c r="A245" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
     </row>
     <row r="246" spans="1:3">
       <c r="A246">
-        <v>2405</v>
+        <v>2401</v>
       </c>
       <c r="B246" t="s">
-        <v>197</v>
+        <v>90</v>
       </c>
       <c r="C246" t="s">
         <v>199</v>
@@ -3482,10 +3494,10 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247">
-        <v>2406</v>
+        <v>2402</v>
       </c>
       <c r="B247" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C247" t="s">
         <v>199</v>
@@ -3493,54 +3505,54 @@
     </row>
     <row r="248" spans="1:3">
       <c r="A248">
-        <v>2407</v>
+        <v>2403</v>
       </c>
       <c r="B248" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
       <c r="C248" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249">
-        <v>2408</v>
+        <v>2404</v>
       </c>
       <c r="B249" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C249" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250">
-        <v>2409</v>
+        <v>2405</v>
       </c>
       <c r="B250" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="C250" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251">
-        <v>2410</v>
+        <v>2406</v>
       </c>
       <c r="B251" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C251" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252">
-        <v>2411</v>
+        <v>2407</v>
       </c>
       <c r="B252" t="s">
-        <v>197</v>
+        <v>90</v>
       </c>
       <c r="C252" t="s">
         <v>200</v>
@@ -3548,17 +3560,77 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253">
-        <v>2412</v>
+        <v>2408</v>
       </c>
       <c r="B253" t="s">
-        <v>202</v>
+        <v>86</v>
       </c>
       <c r="C253" t="s">
         <v>200</v>
       </c>
     </row>
+    <row r="254" spans="1:3">
+      <c r="A254">
+        <v>2409</v>
+      </c>
+      <c r="B254" t="s">
+        <v>120</v>
+      </c>
+      <c r="C254" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255">
+        <v>2410</v>
+      </c>
+      <c r="B255" t="s">
+        <v>201</v>
+      </c>
+      <c r="C255" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256">
+        <v>2411</v>
+      </c>
+      <c r="B256" t="s">
+        <v>197</v>
+      </c>
+      <c r="C256" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257">
+        <v>2412</v>
+      </c>
+      <c r="B257" t="s">
+        <v>202</v>
+      </c>
+      <c r="C257" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A155:C155"/>
+    <mergeCell ref="A229:C229"/>
+    <mergeCell ref="A222:C222"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A210:C210"/>
+    <mergeCell ref="A215:C215"/>
+    <mergeCell ref="A235:C235"/>
+    <mergeCell ref="A173:C173"/>
+    <mergeCell ref="A196:C196"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A99:C99"/>
     <mergeCell ref="A118:C118"/>
     <mergeCell ref="A44:C44"/>
@@ -3566,22 +3638,6 @@
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A241:C241"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A155:C155"/>
-    <mergeCell ref="A230:C230"/>
-    <mergeCell ref="A223:C223"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="A210:C210"/>
-    <mergeCell ref="A216:C216"/>
-    <mergeCell ref="A236:C236"/>
-    <mergeCell ref="A173:C173"/>
-    <mergeCell ref="A196:C196"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>